<commit_message>
🔨 improve converter script
</commit_message>
<xml_diff>
--- a/tools/times.xlsx
+++ b/tools/times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\thi-olympics-scoreboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\thi-olympics-scoreboard\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC9BCF3-6B81-41E9-B3AA-7361A8A28C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD656AF-338F-402C-8E03-30876FAF35D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{76531F41-278F-4E7C-AC39-1D779B36B3A4}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="43">
   <si>
-    <t>BS1</t>
-  </si>
-  <si>
     <t>E1- Team 2</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Pause</t>
+  </si>
+  <si>
+    <t>BS1 - Team 1</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,986 +788,986 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>